<commit_message>
Made highlighted plots of training vs. test data
</commit_message>
<xml_diff>
--- a/Data/Chapter_2_0312.xlsx
+++ b/Data/Chapter_2_0312.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lekro\Documents\Masters\Maps and Data\urban_sprawl_stats\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{870B6AA6-2A00-4A55-B4D9-C57A49E1B308}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE055E27-8486-4C28-BE57-D71BF0BDCFD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{DF1A4302-04C5-447F-8D55-9808EC651F08}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$G$1:$G$197</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$G$1:$G$195</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -135,7 +135,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -155,7 +155,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -470,11 +469,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2953159-1E1A-4742-B02A-0F9B2BE97856}">
-  <dimension ref="A1:H197"/>
+  <dimension ref="A1:G195"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1" activeCellId="1" sqref="D1:D1048576 E1:E1048576"/>
+      <selection pane="bottomLeft" activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -483,7 +482,7 @@
     <col min="4" max="4" width="14.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -505,9 +504,8 @@
       <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="7"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>293</v>
       </c>
@@ -531,7 +529,7 @@
         <v>4.6153846153846156E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>338</v>
       </c>
@@ -551,11 +549,11 @@
         <v>34</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G100" si="0">F3/C3</f>
+        <f t="shared" ref="G3:G195" si="0">F3/C3</f>
         <v>0.35051546391752575</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>343</v>
       </c>
@@ -579,7 +577,7 @@
         <v>9.2715231788079472E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>415</v>
       </c>
@@ -603,7 +601,7 @@
         <v>0.7068965517241379</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>571</v>
       </c>
@@ -627,7 +625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>671</v>
       </c>
@@ -651,7 +649,7 @@
         <v>0.3783783783783784</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>850</v>
       </c>
@@ -675,7 +673,7 @@
         <v>0.94594594594594594</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>1435</v>
       </c>
@@ -699,7 +697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>1612</v>
       </c>
@@ -723,7 +721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>1652</v>
       </c>
@@ -747,7 +745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>1683</v>
       </c>
@@ -771,7 +769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>1722</v>
       </c>
@@ -795,7 +793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>1763</v>
       </c>
@@ -819,7 +817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>1967</v>
       </c>
@@ -843,7 +841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>2186</v>
       </c>
@@ -2893,6 +2891,19 @@
       <c r="C101" s="1">
         <v>53</v>
       </c>
+      <c r="D101">
+        <v>336.87116023454001</v>
+      </c>
+      <c r="E101">
+        <v>28644.966042559601</v>
+      </c>
+      <c r="F101" s="4">
+        <v>46</v>
+      </c>
+      <c r="G101">
+        <f t="shared" si="0"/>
+        <v>0.86792452830188682</v>
+      </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A102" s="1">
@@ -2904,6 +2915,19 @@
       <c r="C102" s="1">
         <v>1</v>
       </c>
+      <c r="D102">
+        <v>998.66927550659</v>
+      </c>
+      <c r="E102">
+        <v>15555.6253339755</v>
+      </c>
+      <c r="F102" s="4">
+        <v>1</v>
+      </c>
+      <c r="G102">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A103" s="1">
@@ -2915,6 +2939,19 @@
       <c r="C103" s="1">
         <v>516</v>
       </c>
+      <c r="D103">
+        <v>284.04196415991498</v>
+      </c>
+      <c r="E103">
+        <v>15555.6253339755</v>
+      </c>
+      <c r="F103" s="4">
+        <v>4</v>
+      </c>
+      <c r="G103">
+        <f t="shared" si="0"/>
+        <v>7.7519379844961239E-3</v>
+      </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A104" s="1">
@@ -2926,6 +2963,19 @@
       <c r="C104" s="1">
         <v>169</v>
       </c>
+      <c r="D104">
+        <v>3030.7953637559299</v>
+      </c>
+      <c r="E104">
+        <v>32384.9124603446</v>
+      </c>
+      <c r="F104" s="4">
+        <v>1</v>
+      </c>
+      <c r="G104">
+        <f t="shared" si="0"/>
+        <v>5.9171597633136093E-3</v>
+      </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A105" s="1">
@@ -2937,6 +2987,19 @@
       <c r="C105" s="1">
         <v>13</v>
       </c>
+      <c r="D105">
+        <v>94.126843060125495</v>
+      </c>
+      <c r="E105">
+        <v>32384.9124603446</v>
+      </c>
+      <c r="F105" s="4">
+        <v>13</v>
+      </c>
+      <c r="G105">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A106" s="1">
@@ -2948,6 +3011,19 @@
       <c r="C106" s="1">
         <v>21</v>
       </c>
+      <c r="D106">
+        <v>16.267730971212099</v>
+      </c>
+      <c r="E106">
+        <v>9350.20602535125</v>
+      </c>
+      <c r="F106" s="4">
+        <v>21</v>
+      </c>
+      <c r="G106">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A107" s="1">
@@ -2959,6 +3035,19 @@
       <c r="C107" s="1">
         <v>19</v>
       </c>
+      <c r="D107">
+        <v>423.39934006530598</v>
+      </c>
+      <c r="E107">
+        <v>6890.2394376807797</v>
+      </c>
+      <c r="F107" s="4">
+        <v>19</v>
+      </c>
+      <c r="G107">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A108" s="1">
@@ -2970,6 +3059,19 @@
       <c r="C108" s="1">
         <v>2</v>
       </c>
+      <c r="D108">
+        <v>3585.4437241943701</v>
+      </c>
+      <c r="E108">
+        <v>10162.060304266</v>
+      </c>
+      <c r="F108" s="4">
+        <v>2</v>
+      </c>
+      <c r="G108">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A109" s="1">
@@ -2981,6 +3083,19 @@
       <c r="C109" s="1">
         <v>5</v>
       </c>
+      <c r="D109">
+        <v>1318.61634588027</v>
+      </c>
+      <c r="E109">
+        <v>7467.2501964728699</v>
+      </c>
+      <c r="F109" s="4">
+        <v>5</v>
+      </c>
+      <c r="G109">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A110" s="1">
@@ -2992,6 +3107,19 @@
       <c r="C110" s="1">
         <v>19</v>
       </c>
+      <c r="D110">
+        <v>1042.8312245644399</v>
+      </c>
+      <c r="E110">
+        <v>11738.159481340899</v>
+      </c>
+      <c r="F110" s="4">
+        <v>19</v>
+      </c>
+      <c r="G110">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A111" s="1">
@@ -3003,6 +3131,19 @@
       <c r="C111" s="1">
         <v>5</v>
       </c>
+      <c r="D111">
+        <v>225.252328922207</v>
+      </c>
+      <c r="E111">
+        <v>10162.060304266</v>
+      </c>
+      <c r="F111" s="4">
+        <v>5</v>
+      </c>
+      <c r="G111">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A112" s="1">
@@ -3014,8 +3155,21 @@
       <c r="C112" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D112">
+        <v>1105.54167209768</v>
+      </c>
+      <c r="E112">
+        <v>6669.4888425254503</v>
+      </c>
+      <c r="F112" s="4">
+        <v>10</v>
+      </c>
+      <c r="G112">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A113" s="1">
         <v>20197</v>
       </c>
@@ -3025,8 +3179,21 @@
       <c r="C113" s="1">
         <v>9</v>
       </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D113">
+        <v>35.534697549179498</v>
+      </c>
+      <c r="E113">
+        <v>6669.4888425254503</v>
+      </c>
+      <c r="F113" s="4">
+        <v>9</v>
+      </c>
+      <c r="G113">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A114" s="1">
         <v>20256</v>
       </c>
@@ -3036,8 +3203,21 @@
       <c r="C114" s="1">
         <v>11</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D114">
+        <v>28.5973871363359</v>
+      </c>
+      <c r="E114">
+        <v>31049.119934331899</v>
+      </c>
+      <c r="F114" s="4">
+        <v>11</v>
+      </c>
+      <c r="G114">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A115" s="1">
         <v>20311</v>
       </c>
@@ -3047,8 +3227,21 @@
       <c r="C115" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D115">
+        <v>864.87473713451197</v>
+      </c>
+      <c r="E115">
+        <v>13609.743490089701</v>
+      </c>
+      <c r="F115" s="4">
+        <v>15</v>
+      </c>
+      <c r="G115">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A116" s="1">
         <v>20344</v>
       </c>
@@ -3058,8 +3251,21 @@
       <c r="C116" s="1">
         <v>152</v>
       </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D116">
+        <v>523.86844420689602</v>
+      </c>
+      <c r="E116">
+        <v>13435.457842378801</v>
+      </c>
+      <c r="F116" s="4">
+        <v>2</v>
+      </c>
+      <c r="G116">
+        <f t="shared" si="0"/>
+        <v>1.3157894736842105E-2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A117" s="1">
         <v>20497</v>
       </c>
@@ -3069,8 +3275,21 @@
       <c r="C117" s="1">
         <v>18</v>
       </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D117">
+        <v>610.685518009048</v>
+      </c>
+      <c r="E117">
+        <v>6153.9357461703103</v>
+      </c>
+      <c r="F117" s="4">
+        <v>18</v>
+      </c>
+      <c r="G117">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A118" s="1">
         <v>20614</v>
       </c>
@@ -3080,8 +3299,21 @@
       <c r="C118" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D118">
+        <v>1418.7381937471901</v>
+      </c>
+      <c r="E118">
+        <v>32034.151119972601</v>
+      </c>
+      <c r="F118" s="4">
+        <v>15</v>
+      </c>
+      <c r="G118">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A119" s="1">
         <v>20797</v>
       </c>
@@ -3091,8 +3323,21 @@
       <c r="C119" s="1">
         <v>92</v>
       </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D119">
+        <v>135.45317064309</v>
+      </c>
+      <c r="E119">
+        <v>1638388.56948889</v>
+      </c>
+      <c r="F119" s="4">
+        <v>38</v>
+      </c>
+      <c r="G119">
+        <f t="shared" si="0"/>
+        <v>0.41304347826086957</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A120" s="1">
         <v>21145</v>
       </c>
@@ -3102,8 +3347,21 @@
       <c r="C120" s="1">
         <v>160</v>
       </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D120">
+        <v>151.876757803494</v>
+      </c>
+      <c r="E120">
+        <v>17271.057098743298</v>
+      </c>
+      <c r="F120" s="4">
+        <v>61</v>
+      </c>
+      <c r="G120">
+        <f t="shared" si="0"/>
+        <v>0.38124999999999998</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A121" s="1">
         <v>21169</v>
       </c>
@@ -3113,8 +3371,21 @@
       <c r="C121" s="1">
         <v>132</v>
       </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D121">
+        <v>556.11097194165302</v>
+      </c>
+      <c r="E121">
+        <v>11297.733044295799</v>
+      </c>
+      <c r="F121" s="4">
+        <v>45</v>
+      </c>
+      <c r="G121">
+        <f t="shared" si="0"/>
+        <v>0.34090909090909088</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A122" s="1">
         <v>21694</v>
       </c>
@@ -3124,8 +3395,21 @@
       <c r="C122" s="1">
         <v>47</v>
       </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D122">
+        <v>1203.56571747871</v>
+      </c>
+      <c r="E122">
+        <v>1638388.56948889</v>
+      </c>
+      <c r="F122" s="4">
+        <v>19</v>
+      </c>
+      <c r="G122">
+        <f t="shared" si="0"/>
+        <v>0.40425531914893614</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A123" s="1">
         <v>21712</v>
       </c>
@@ -3133,10 +3417,23 @@
         <v>0.132016010020785</v>
       </c>
       <c r="C123" s="1">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.35">
+        <v>98</v>
+      </c>
+      <c r="D123">
+        <v>382.92441053418901</v>
+      </c>
+      <c r="E123">
+        <v>48085.110135964198</v>
+      </c>
+      <c r="F123" s="4">
+        <v>28</v>
+      </c>
+      <c r="G123">
+        <f t="shared" si="0"/>
+        <v>0.2857142857142857</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A124" s="1">
         <v>21888</v>
       </c>
@@ -3146,8 +3443,21 @@
       <c r="C124" s="1">
         <v>133</v>
       </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D124">
+        <v>681.76053150440305</v>
+      </c>
+      <c r="E124">
+        <v>53250.213016576097</v>
+      </c>
+      <c r="F124" s="4">
+        <v>24</v>
+      </c>
+      <c r="G124">
+        <f t="shared" si="0"/>
+        <v>0.18045112781954886</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A125" s="1">
         <v>21949</v>
       </c>
@@ -3157,8 +3467,21 @@
       <c r="C125" s="1">
         <v>260</v>
       </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D125">
+        <v>278.33773644366698</v>
+      </c>
+      <c r="E125">
+        <v>54668.8966663725</v>
+      </c>
+      <c r="F125" s="4">
+        <v>21</v>
+      </c>
+      <c r="G125">
+        <f t="shared" si="0"/>
+        <v>8.0769230769230774E-2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A126" s="1">
         <v>22102</v>
       </c>
@@ -3168,8 +3491,21 @@
       <c r="C126" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D126">
+        <v>1035.6794895032999</v>
+      </c>
+      <c r="E126">
+        <v>5614.8385571054996</v>
+      </c>
+      <c r="F126" s="4">
+        <v>20</v>
+      </c>
+      <c r="G126">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A127" s="1">
         <v>22979</v>
       </c>
@@ -3179,8 +3515,21 @@
       <c r="C127" s="1">
         <v>14</v>
       </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D127">
+        <v>1742.1040713616901</v>
+      </c>
+      <c r="E127">
+        <v>20425.621651785401</v>
+      </c>
+      <c r="F127" s="4">
+        <v>13</v>
+      </c>
+      <c r="G127">
+        <f t="shared" si="0"/>
+        <v>0.9285714285714286</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A128" s="1">
         <v>23286</v>
       </c>
@@ -3190,8 +3539,21 @@
       <c r="C128" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D128">
+        <v>1467.13751683495</v>
+      </c>
+      <c r="E128">
+        <v>37798.923818287301</v>
+      </c>
+      <c r="F128" s="4">
+        <v>5</v>
+      </c>
+      <c r="G128">
+        <f t="shared" si="0"/>
+        <v>0.7142857142857143</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A129" s="1">
         <v>23456</v>
       </c>
@@ -3201,8 +3563,21 @@
       <c r="C129" s="1">
         <v>168</v>
       </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D129">
+        <v>150.87011516956201</v>
+      </c>
+      <c r="E129">
+        <v>16575.360250020702</v>
+      </c>
+      <c r="F129" s="4">
+        <v>12</v>
+      </c>
+      <c r="G129">
+        <f t="shared" si="0"/>
+        <v>7.1428571428571425E-2</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A130" s="1">
         <v>23782</v>
       </c>
@@ -3212,8 +3587,21 @@
       <c r="C130" s="1">
         <v>19</v>
       </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D130">
+        <v>994.17513624591504</v>
+      </c>
+      <c r="E130">
+        <v>33015.159322473803</v>
+      </c>
+      <c r="F130" s="4">
+        <v>2</v>
+      </c>
+      <c r="G130">
+        <f t="shared" si="0"/>
+        <v>0.10526315789473684</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A131" s="1">
         <v>24054</v>
       </c>
@@ -3223,8 +3611,21 @@
       <c r="C131" s="1">
         <v>47</v>
       </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D131">
+        <v>92.238123150886096</v>
+      </c>
+      <c r="E131">
+        <v>15791.0239577302</v>
+      </c>
+      <c r="F131" s="4">
+        <v>30</v>
+      </c>
+      <c r="G131">
+        <f t="shared" si="0"/>
+        <v>0.63829787234042556</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A132" s="1">
         <v>24147</v>
       </c>
@@ -3234,8 +3635,21 @@
       <c r="C132" s="1">
         <v>49</v>
       </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D132">
+        <v>348.437254453386</v>
+      </c>
+      <c r="E132">
+        <v>46545.7833567993</v>
+      </c>
+      <c r="F132" s="4">
+        <v>39</v>
+      </c>
+      <c r="G132">
+        <f t="shared" si="0"/>
+        <v>0.79591836734693877</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A133" s="1">
         <v>24745</v>
       </c>
@@ -3245,8 +3659,21 @@
       <c r="C133" s="1">
         <v>30</v>
       </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D133">
+        <v>193.34804004967901</v>
+      </c>
+      <c r="E133">
+        <v>7715.9664918117496</v>
+      </c>
+      <c r="F133" s="4">
+        <v>30</v>
+      </c>
+      <c r="G133">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A134" s="1">
         <v>24751</v>
       </c>
@@ -3256,8 +3683,21 @@
       <c r="C134" s="1">
         <v>25</v>
       </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D134">
+        <v>134.970052478112</v>
+      </c>
+      <c r="E134">
+        <v>5002.7402202891599</v>
+      </c>
+      <c r="F134" s="4">
+        <v>14</v>
+      </c>
+      <c r="G134">
+        <f t="shared" si="0"/>
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A135" s="1">
         <v>24769</v>
       </c>
@@ -3267,8 +3707,21 @@
       <c r="C135" s="1">
         <v>13</v>
       </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D135">
+        <v>48.889198673332999</v>
+      </c>
+      <c r="E135">
+        <v>7715.9664918117496</v>
+      </c>
+      <c r="F135" s="4">
+        <v>13</v>
+      </c>
+      <c r="G135">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A136" s="1">
         <v>26257</v>
       </c>
@@ -3278,8 +3731,21 @@
       <c r="C136" s="1">
         <v>30</v>
       </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D136">
+        <v>557.085569498616</v>
+      </c>
+      <c r="E136">
+        <v>12424.1815162611</v>
+      </c>
+      <c r="F136" s="4">
+        <v>30</v>
+      </c>
+      <c r="G136">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A137" s="1">
         <v>26324</v>
       </c>
@@ -3289,8 +3755,21 @@
       <c r="C137" s="1">
         <v>31</v>
       </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D137">
+        <v>529.376538747479</v>
+      </c>
+      <c r="E137">
+        <v>8978.7176547829804</v>
+      </c>
+      <c r="F137" s="4">
+        <v>31</v>
+      </c>
+      <c r="G137">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A138" s="1">
         <v>26900</v>
       </c>
@@ -3300,8 +3779,21 @@
       <c r="C138" s="1">
         <v>126</v>
       </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D138">
+        <v>11.148934229745301</v>
+      </c>
+      <c r="E138">
+        <v>264774.92073005601</v>
+      </c>
+      <c r="F138" s="4">
+        <v>19</v>
+      </c>
+      <c r="G138">
+        <f t="shared" si="0"/>
+        <v>0.15079365079365079</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A139" s="1">
         <v>27023</v>
       </c>
@@ -3311,8 +3803,21 @@
       <c r="C139" s="1">
         <v>36</v>
       </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D139">
+        <v>103.983004401461</v>
+      </c>
+      <c r="E139">
+        <v>5134.7985334551604</v>
+      </c>
+      <c r="F139" s="4">
+        <v>30</v>
+      </c>
+      <c r="G139">
+        <f t="shared" si="0"/>
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A140" s="1">
         <v>27502</v>
       </c>
@@ -3322,8 +3827,21 @@
       <c r="C140" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D140">
+        <v>187.088714117764</v>
+      </c>
+      <c r="E140">
+        <v>5694.2831667126302</v>
+      </c>
+      <c r="F140" s="4">
+        <v>2</v>
+      </c>
+      <c r="G140">
+        <f t="shared" si="0"/>
+        <v>0.2857142857142857</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A141" s="1">
         <v>27557</v>
       </c>
@@ -3333,8 +3851,21 @@
       <c r="C141" s="1">
         <v>9</v>
       </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D141">
+        <v>186.02072026192499</v>
+      </c>
+      <c r="E141">
+        <v>5694.2831667126302</v>
+      </c>
+      <c r="F141" s="4">
+        <v>4</v>
+      </c>
+      <c r="G141">
+        <f t="shared" si="0"/>
+        <v>0.44444444444444442</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A142" s="1">
         <v>27652</v>
       </c>
@@ -3344,8 +3875,21 @@
       <c r="C142" s="1">
         <v>30</v>
       </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D142">
+        <v>561.71469594200403</v>
+      </c>
+      <c r="E142">
+        <v>5694.2831667126302</v>
+      </c>
+      <c r="F142" s="4">
+        <v>4</v>
+      </c>
+      <c r="G142">
+        <f t="shared" si="0"/>
+        <v>0.13333333333333333</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A143" s="1">
         <v>27682</v>
       </c>
@@ -3353,10 +3897,23 @@
         <v>7.9047146952302E-2</v>
       </c>
       <c r="C143" s="1">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+      <c r="D143">
+        <v>833.01858323196495</v>
+      </c>
+      <c r="E143">
+        <v>5694.2831667126302</v>
+      </c>
+      <c r="F143" s="4">
+        <v>12</v>
+      </c>
+      <c r="G143">
+        <f t="shared" si="0"/>
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A144" s="1">
         <v>27863</v>
       </c>
@@ -3366,8 +3923,21 @@
       <c r="C144" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D144">
+        <v>1189.6854570488999</v>
+      </c>
+      <c r="E144">
+        <v>9345.6041483756999</v>
+      </c>
+      <c r="F144" s="4">
+        <v>2</v>
+      </c>
+      <c r="G144">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A145" s="1">
         <v>28695</v>
       </c>
@@ -3377,8 +3947,21 @@
       <c r="C145" s="1">
         <v>247</v>
       </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D145">
+        <v>1116.86385114532</v>
+      </c>
+      <c r="E145">
+        <v>8842.1053993253699</v>
+      </c>
+      <c r="F145" s="4">
+        <v>54</v>
+      </c>
+      <c r="G145">
+        <f t="shared" si="0"/>
+        <v>0.21862348178137653</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A146" s="1">
         <v>28741</v>
       </c>
@@ -3388,8 +3971,21 @@
       <c r="C146" s="1">
         <v>287</v>
       </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D146">
+        <v>879.99524565505999</v>
+      </c>
+      <c r="E146">
+        <v>8842.1053993253699</v>
+      </c>
+      <c r="F146" s="4">
+        <v>66</v>
+      </c>
+      <c r="G146">
+        <f t="shared" si="0"/>
+        <v>0.22996515679442509</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A147" s="1">
         <v>28931</v>
       </c>
@@ -3399,559 +3995,1174 @@
       <c r="C147" s="1">
         <v>422</v>
       </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D147">
+        <v>209.067407523632</v>
+      </c>
+      <c r="E147">
+        <v>195447.86973925901</v>
+      </c>
+      <c r="F147" s="4">
+        <v>7</v>
+      </c>
+      <c r="G147">
+        <f t="shared" si="0"/>
+        <v>1.6587677725118485E-2</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A148" s="1">
-        <v>28941</v>
+        <v>29176</v>
       </c>
       <c r="B148" s="1">
-        <v>5.0670001873741002E-2</v>
+        <v>0</v>
       </c>
       <c r="C148" s="1">
-        <v>3228</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="D148">
+        <v>531.61891187391097</v>
+      </c>
+      <c r="E148">
+        <v>78787.622770918402</v>
+      </c>
+      <c r="F148" s="4">
+        <v>1</v>
+      </c>
+      <c r="G148">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A149" s="1">
-        <v>29176</v>
+        <v>29356</v>
       </c>
       <c r="B149" s="1">
+        <v>3.9836308256170003E-2</v>
+      </c>
+      <c r="C149" s="1">
+        <v>7</v>
+      </c>
+      <c r="D149">
+        <v>161.44326414446999</v>
+      </c>
+      <c r="E149">
+        <v>8888.2382449069792</v>
+      </c>
+      <c r="F149" s="4">
+        <v>7</v>
+      </c>
+      <c r="G149">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A150" s="1">
+        <v>29470</v>
+      </c>
+      <c r="B150" s="1">
+        <v>5.1079411437754997E-2</v>
+      </c>
+      <c r="C150" s="1">
+        <v>10</v>
+      </c>
+      <c r="D150">
+        <v>397.89655482959103</v>
+      </c>
+      <c r="E150">
+        <v>8888.2382449069792</v>
+      </c>
+      <c r="F150" s="4">
+        <v>10</v>
+      </c>
+      <c r="G150">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A151" s="1">
+        <v>30086</v>
+      </c>
+      <c r="B151" s="1">
+        <v>0.25883072194665302</v>
+      </c>
+      <c r="C151" s="1">
+        <v>155</v>
+      </c>
+      <c r="D151">
+        <v>517.49456785501195</v>
+      </c>
+      <c r="E151">
+        <v>7867.0045987517096</v>
+      </c>
+      <c r="F151" s="4">
+        <v>36</v>
+      </c>
+      <c r="G151">
+        <f t="shared" si="0"/>
+        <v>0.23225806451612904</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A152" s="1">
+        <v>30382</v>
+      </c>
+      <c r="B152" s="1">
+        <v>0.57673259965957202</v>
+      </c>
+      <c r="C152" s="1">
+        <v>254</v>
+      </c>
+      <c r="D152">
+        <v>1140.4378232750701</v>
+      </c>
+      <c r="E152">
+        <v>11858.6619097284</v>
+      </c>
+      <c r="F152" s="4">
         <v>0</v>
       </c>
-      <c r="C149" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A150" s="1">
-        <v>29356</v>
-      </c>
-      <c r="B150" s="1">
-        <v>3.9836308256170003E-2</v>
-      </c>
-      <c r="C150" s="1">
+      <c r="G152">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A153" s="1">
+        <v>30445</v>
+      </c>
+      <c r="B153" s="1">
+        <v>0.48191837277606198</v>
+      </c>
+      <c r="C153" s="1">
+        <v>35</v>
+      </c>
+      <c r="D153">
+        <v>119.578829097888</v>
+      </c>
+      <c r="E153">
+        <v>5522.4228259915399</v>
+      </c>
+      <c r="F153" s="4">
+        <v>0</v>
+      </c>
+      <c r="G153">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A154" s="1">
+        <v>30628</v>
+      </c>
+      <c r="B154" s="1">
+        <v>3.3039573627447999E-2</v>
+      </c>
+      <c r="C154" s="1">
+        <v>27</v>
+      </c>
+      <c r="D154">
+        <v>464.92211360342799</v>
+      </c>
+      <c r="E154">
+        <v>5522.4228259915399</v>
+      </c>
+      <c r="F154" s="4">
+        <v>8</v>
+      </c>
+      <c r="G154">
+        <f t="shared" si="0"/>
+        <v>0.29629629629629628</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A155" s="1">
+        <v>31231</v>
+      </c>
+      <c r="B155" s="1">
+        <v>0.32213241998207898</v>
+      </c>
+      <c r="C155" s="1">
+        <v>158</v>
+      </c>
+      <c r="D155">
+        <v>221.26113182004201</v>
+      </c>
+      <c r="E155">
+        <v>11621.405460166599</v>
+      </c>
+      <c r="F155" s="4">
+        <v>41</v>
+      </c>
+      <c r="G155">
+        <f t="shared" si="0"/>
+        <v>0.25949367088607594</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A156" s="1">
+        <v>32010</v>
+      </c>
+      <c r="B156" s="1">
+        <v>0.136181609714949</v>
+      </c>
+      <c r="C156" s="1">
+        <v>65</v>
+      </c>
+      <c r="D156">
+        <v>1576.8420758459099</v>
+      </c>
+      <c r="E156">
+        <v>7404.1731147351002</v>
+      </c>
+      <c r="F156" s="4">
+        <v>5</v>
+      </c>
+      <c r="G156">
+        <f t="shared" si="0"/>
+        <v>7.6923076923076927E-2</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A157" s="1">
+        <v>32145</v>
+      </c>
+      <c r="B157" s="1">
+        <v>0.26118896032327898</v>
+      </c>
+      <c r="C157" s="1">
+        <v>112</v>
+      </c>
+      <c r="D157">
+        <v>697.89834796480704</v>
+      </c>
+      <c r="E157">
+        <v>31458.3222520977</v>
+      </c>
+      <c r="F157" s="4">
+        <v>30</v>
+      </c>
+      <c r="G157">
+        <f t="shared" si="0"/>
+        <v>0.26785714285714285</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A158" s="1">
+        <v>32923</v>
+      </c>
+      <c r="B158" s="1">
+        <v>3.3038622127386001E-2</v>
+      </c>
+      <c r="C158" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A151" s="1">
-        <v>29470</v>
-      </c>
-      <c r="B151" s="1">
-        <v>5.1079411437754997E-2</v>
-      </c>
-      <c r="C151" s="1">
+      <c r="D158">
+        <v>928.37293077065601</v>
+      </c>
+      <c r="E158">
+        <v>7781.3885680410103</v>
+      </c>
+      <c r="F158" s="4">
+        <v>7</v>
+      </c>
+      <c r="G158">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A159" s="1">
+        <v>33224</v>
+      </c>
+      <c r="B159" s="1">
+        <v>8.8011013180742004E-2</v>
+      </c>
+      <c r="C159" s="1">
+        <v>29</v>
+      </c>
+      <c r="D159">
+        <v>36.498439940802697</v>
+      </c>
+      <c r="E159">
+        <v>70453.920465390998</v>
+      </c>
+      <c r="F159" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A152" s="1">
-        <v>30086</v>
-      </c>
-      <c r="B152" s="1">
-        <v>0.25883072194665302</v>
-      </c>
-      <c r="C152" s="1">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A153" s="1">
-        <v>30382</v>
-      </c>
-      <c r="B153" s="1">
-        <v>0.57673259965957202</v>
-      </c>
-      <c r="C153" s="1">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A154" s="1">
-        <v>30445</v>
-      </c>
-      <c r="B154" s="1">
-        <v>0.48191837277606198</v>
-      </c>
-      <c r="C154" s="1">
+      <c r="G159">
+        <f t="shared" si="0"/>
+        <v>0.34482758620689657</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A160" s="1">
+        <v>33327</v>
+      </c>
+      <c r="B160" s="1">
+        <v>0.178798741068562</v>
+      </c>
+      <c r="C160" s="1">
+        <v>42</v>
+      </c>
+      <c r="D160">
+        <v>162.87572488484801</v>
+      </c>
+      <c r="E160">
+        <v>71785.895035361798</v>
+      </c>
+      <c r="F160" s="4">
+        <v>19</v>
+      </c>
+      <c r="G160">
+        <f t="shared" si="0"/>
+        <v>0.45238095238095238</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A161" s="1">
+        <v>33340</v>
+      </c>
+      <c r="B161" s="1">
+        <v>0.18296331444587</v>
+      </c>
+      <c r="C161" s="1">
+        <v>94</v>
+      </c>
+      <c r="D161">
+        <v>116.383278801828</v>
+      </c>
+      <c r="E161">
+        <v>21612.703632219302</v>
+      </c>
+      <c r="F161" s="4">
+        <v>18</v>
+      </c>
+      <c r="G161">
+        <f t="shared" si="0"/>
+        <v>0.19148936170212766</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A162" s="1">
+        <v>33411</v>
+      </c>
+      <c r="B162" s="1">
+        <v>0.21607189799624801</v>
+      </c>
+      <c r="C162" s="1">
+        <v>118</v>
+      </c>
+      <c r="D162">
+        <v>485.26498276493402</v>
+      </c>
+      <c r="E162">
+        <v>21612.703632219302</v>
+      </c>
+      <c r="F162" s="4">
+        <v>34</v>
+      </c>
+      <c r="G162">
+        <f t="shared" si="0"/>
+        <v>0.28813559322033899</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A163" s="1">
+        <v>33444</v>
+      </c>
+      <c r="B163" s="1">
+        <v>0.172066365078858</v>
+      </c>
+      <c r="C163" s="1">
+        <v>83</v>
+      </c>
+      <c r="D163">
+        <v>916.51634091244296</v>
+      </c>
+      <c r="E163">
+        <v>9223.6399455093106</v>
+      </c>
+      <c r="F163" s="4">
+        <v>25</v>
+      </c>
+      <c r="G163">
+        <f t="shared" si="0"/>
+        <v>0.30120481927710846</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A164" s="1">
+        <v>33594</v>
+      </c>
+      <c r="B164" s="1">
+        <v>0.111333339450349</v>
+      </c>
+      <c r="C164" s="1">
+        <v>34</v>
+      </c>
+      <c r="D164">
+        <v>1039.2665599048</v>
+      </c>
+      <c r="E164">
+        <v>9350.8579017630309</v>
+      </c>
+      <c r="F164" s="4">
+        <v>27</v>
+      </c>
+      <c r="G164">
+        <f t="shared" si="0"/>
+        <v>0.79411764705882348</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A165" s="1">
+        <v>33724</v>
+      </c>
+      <c r="B165" s="1">
+        <v>0.17067917439993199</v>
+      </c>
+      <c r="C165" s="1">
+        <v>37</v>
+      </c>
+      <c r="D165">
+        <v>463.29436257755998</v>
+      </c>
+      <c r="E165">
+        <v>24380.4663917012</v>
+      </c>
+      <c r="F165" s="4">
+        <v>37</v>
+      </c>
+      <c r="G165">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A166" s="1">
+        <v>33993</v>
+      </c>
+      <c r="B166" s="1">
+        <v>8.8290035277060003E-2</v>
+      </c>
+      <c r="C166" s="1">
+        <v>22</v>
+      </c>
+      <c r="D166">
+        <v>112.422678654907</v>
+      </c>
+      <c r="E166">
+        <v>35665.548591509199</v>
+      </c>
+      <c r="F166" s="4">
+        <v>21</v>
+      </c>
+      <c r="G166">
+        <f t="shared" si="0"/>
+        <v>0.95454545454545459</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A167" s="1">
+        <v>34175</v>
+      </c>
+      <c r="B167" s="1">
+        <v>9.3843243701032003E-2</v>
+      </c>
+      <c r="C167" s="1">
+        <v>29</v>
+      </c>
+      <c r="D167">
+        <v>5.6941782652557098</v>
+      </c>
+      <c r="E167">
+        <v>66523.128691095597</v>
+      </c>
+      <c r="F167" s="4">
+        <v>29</v>
+      </c>
+      <c r="G167">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A168" s="1">
+        <v>34259</v>
+      </c>
+      <c r="B168" s="1">
+        <v>0</v>
+      </c>
+      <c r="C168" s="1">
+        <v>4</v>
+      </c>
+      <c r="D168">
+        <v>658.85382439311797</v>
+      </c>
+      <c r="E168">
+        <v>66523.128691095597</v>
+      </c>
+      <c r="F168" s="4">
+        <v>4</v>
+      </c>
+      <c r="G168">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A169" s="1">
+        <v>34261</v>
+      </c>
+      <c r="B169" s="1">
+        <v>0.137780482898372</v>
+      </c>
+      <c r="C169" s="1">
+        <v>26</v>
+      </c>
+      <c r="D169">
+        <v>856.64005057864995</v>
+      </c>
+      <c r="E169">
+        <v>66523.128691095597</v>
+      </c>
+      <c r="F169" s="4">
+        <v>26</v>
+      </c>
+      <c r="G169">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A170" s="1">
+        <v>34478</v>
+      </c>
+      <c r="B170" s="1">
+        <v>8.1211043079211995E-2</v>
+      </c>
+      <c r="C170" s="1">
+        <v>27</v>
+      </c>
+      <c r="D170">
+        <v>1097.49346609188</v>
+      </c>
+      <c r="E170">
+        <v>9419.6022476391408</v>
+      </c>
+      <c r="F170" s="4">
+        <v>27</v>
+      </c>
+      <c r="G170">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A171" s="1">
+        <v>34559</v>
+      </c>
+      <c r="B171" s="1">
+        <v>1.8046923079220001E-3</v>
+      </c>
+      <c r="C171" s="1">
+        <v>6</v>
+      </c>
+      <c r="D171">
+        <v>1528.0953121776399</v>
+      </c>
+      <c r="E171">
+        <v>9419.6022476391408</v>
+      </c>
+      <c r="F171" s="4">
+        <v>2</v>
+      </c>
+      <c r="G171">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A172" s="1">
+        <v>34938</v>
+      </c>
+      <c r="B172" s="1">
+        <v>7.5033906778769005E-2</v>
+      </c>
+      <c r="C172" s="1">
+        <v>12</v>
+      </c>
+      <c r="D172">
+        <v>2173.42952029252</v>
+      </c>
+      <c r="E172" s="3">
+        <v>7871.55826412634</v>
+      </c>
+      <c r="F172" s="4">
+        <v>11</v>
+      </c>
+      <c r="G172">
+        <f t="shared" si="0"/>
+        <v>0.91666666666666663</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A173" s="1">
+        <v>35028</v>
+      </c>
+      <c r="B173" s="1">
+        <v>1.7977621312515998E-2</v>
+      </c>
+      <c r="C173" s="1">
+        <v>1</v>
+      </c>
+      <c r="D173">
+        <v>9.3304758846237004</v>
+      </c>
+      <c r="E173">
+        <v>40792.401587032997</v>
+      </c>
+      <c r="F173" s="4">
+        <v>1</v>
+      </c>
+      <c r="G173">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A174" s="1">
+        <v>35571</v>
+      </c>
+      <c r="B174" s="1">
+        <v>0.17491835876145401</v>
+      </c>
+      <c r="C174" s="1">
+        <v>38</v>
+      </c>
+      <c r="D174">
+        <v>91.351517323016395</v>
+      </c>
+      <c r="E174">
+        <v>5661.1650250975599</v>
+      </c>
+      <c r="F174" s="4">
+        <v>38</v>
+      </c>
+      <c r="G174">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A175" s="1">
+        <v>35687</v>
+      </c>
+      <c r="B175" s="1">
+        <v>0.14465490386308799</v>
+      </c>
+      <c r="C175" s="1">
+        <v>47</v>
+      </c>
+      <c r="D175">
+        <v>387.59525052032302</v>
+      </c>
+      <c r="E175">
+        <v>6710.9822826156997</v>
+      </c>
+      <c r="F175" s="4">
+        <v>36</v>
+      </c>
+      <c r="G175">
+        <f t="shared" si="0"/>
+        <v>0.76595744680851063</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A176" s="1">
+        <v>35696</v>
+      </c>
+      <c r="B176" s="1">
+        <v>0.14972198637044401</v>
+      </c>
+      <c r="C176" s="1">
         <v>35</v>
       </c>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A155" s="1">
-        <v>30628</v>
-      </c>
-      <c r="B155" s="1">
-        <v>3.3039573627447999E-2</v>
-      </c>
-      <c r="C155" s="1">
+      <c r="D176">
+        <v>42.801302274377299</v>
+      </c>
+      <c r="E176">
+        <v>19892.073233965199</v>
+      </c>
+      <c r="F176" s="4">
+        <v>31</v>
+      </c>
+      <c r="G176">
+        <f t="shared" si="0"/>
+        <v>0.88571428571428568</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A177" s="1">
+        <v>35880</v>
+      </c>
+      <c r="B177" s="1">
+        <v>0.19317438993014999</v>
+      </c>
+      <c r="C177" s="1">
+        <v>92</v>
+      </c>
+      <c r="D177">
+        <v>490.88273187191498</v>
+      </c>
+      <c r="E177">
+        <v>50276.661202644798</v>
+      </c>
+      <c r="F177" s="4">
+        <v>36</v>
+      </c>
+      <c r="G177">
+        <f t="shared" si="0"/>
+        <v>0.39130434782608697</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A178" s="1">
+        <v>36067</v>
+      </c>
+      <c r="B178" s="1">
+        <v>0.13188361426071599</v>
+      </c>
+      <c r="C178" s="1">
+        <v>32</v>
+      </c>
+      <c r="D178">
+        <v>81.1231585323914</v>
+      </c>
+      <c r="E178">
+        <v>6327.6022110470703</v>
+      </c>
+      <c r="F178" s="4">
+        <v>32</v>
+      </c>
+      <c r="G178">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A179" s="1">
+        <v>36116</v>
+      </c>
+      <c r="B179" s="1">
+        <v>0.139727217499582</v>
+      </c>
+      <c r="C179" s="1">
+        <v>85</v>
+      </c>
+      <c r="D179">
+        <v>1120.9276066357199</v>
+      </c>
+      <c r="E179">
+        <v>37798.923818287301</v>
+      </c>
+      <c r="F179" s="4">
+        <v>14</v>
+      </c>
+      <c r="G179">
+        <f t="shared" si="0"/>
+        <v>0.16470588235294117</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A180" s="1">
+        <v>36462</v>
+      </c>
+      <c r="B180" s="1">
+        <v>2.1240321393725E-2</v>
+      </c>
+      <c r="C180" s="1">
+        <v>3</v>
+      </c>
+      <c r="D180">
+        <v>489.983893899745</v>
+      </c>
+      <c r="E180">
+        <v>18906.7998683968</v>
+      </c>
+      <c r="F180" s="4">
+        <v>3</v>
+      </c>
+      <c r="G180">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A181" s="1">
+        <v>36734</v>
+      </c>
+      <c r="B181" s="1">
+        <v>0.15005624460401901</v>
+      </c>
+      <c r="C181" s="1">
+        <v>33</v>
+      </c>
+      <c r="D181">
+        <v>338.17327412619102</v>
+      </c>
+      <c r="E181">
+        <v>19893.947557728399</v>
+      </c>
+      <c r="F181" s="4">
+        <v>31</v>
+      </c>
+      <c r="G181">
+        <f t="shared" si="0"/>
+        <v>0.93939393939393945</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A182" s="1">
+        <v>36795</v>
+      </c>
+      <c r="B182" s="1">
+        <v>0.102513106267262</v>
+      </c>
+      <c r="C182" s="1">
         <v>27</v>
       </c>
-    </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A156" s="1">
-        <v>31231</v>
-      </c>
-      <c r="B156" s="1">
-        <v>0.32213241998207898</v>
-      </c>
-      <c r="C156" s="1">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A157" s="1">
-        <v>32010</v>
-      </c>
-      <c r="B157" s="1">
-        <v>0.136181609714949</v>
-      </c>
-      <c r="C157" s="1">
+      <c r="D182">
+        <v>865.22911801513101</v>
+      </c>
+      <c r="E182">
+        <v>40848.931740028696</v>
+      </c>
+      <c r="F182" s="4">
+        <v>27</v>
+      </c>
+      <c r="G182">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A183" s="1">
+        <v>36836</v>
+      </c>
+      <c r="B183" s="1">
+        <v>0.13263552081795699</v>
+      </c>
+      <c r="C183" s="1">
+        <v>54</v>
+      </c>
+      <c r="D183">
+        <v>515.00336433607504</v>
+      </c>
+      <c r="E183">
+        <v>40848.931740028696</v>
+      </c>
+      <c r="F183" s="4">
+        <v>21</v>
+      </c>
+      <c r="G183">
+        <f t="shared" si="0"/>
+        <v>0.3888888888888889</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A184" s="1">
+        <v>36909</v>
+      </c>
+      <c r="B184" s="1">
+        <v>0.110217403406246</v>
+      </c>
+      <c r="C184" s="1">
+        <v>46</v>
+      </c>
+      <c r="D184">
+        <v>18.503015533040301</v>
+      </c>
+      <c r="E184">
+        <v>6129.4178897561396</v>
+      </c>
+      <c r="F184" s="4">
+        <v>10</v>
+      </c>
+      <c r="G184">
+        <f t="shared" si="0"/>
+        <v>0.21739130434782608</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A185" s="1">
+        <v>37163</v>
+      </c>
+      <c r="B185" s="1">
+        <v>0.24264602874948901</v>
+      </c>
+      <c r="C185" s="1">
+        <v>304</v>
+      </c>
+      <c r="D185">
+        <v>1683.7724315901401</v>
+      </c>
+      <c r="E185">
+        <v>19665.477716506299</v>
+      </c>
+      <c r="F185" s="4">
+        <v>45</v>
+      </c>
+      <c r="G185">
+        <f t="shared" si="0"/>
+        <v>0.14802631578947367</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A186" s="1">
+        <v>37232</v>
+      </c>
+      <c r="B186" s="1">
+        <v>0.26548117389012899</v>
+      </c>
+      <c r="C186" s="1">
+        <v>78</v>
+      </c>
+      <c r="D186">
+        <v>547.87137954403204</v>
+      </c>
+      <c r="E186">
+        <v>19665.477716506299</v>
+      </c>
+      <c r="F186" s="4">
+        <v>49</v>
+      </c>
+      <c r="G186">
+        <f t="shared" si="0"/>
+        <v>0.62820512820512819</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A187" s="1">
+        <v>37263</v>
+      </c>
+      <c r="B187" s="1">
+        <v>0.12555705320819499</v>
+      </c>
+      <c r="C187" s="1">
+        <v>42</v>
+      </c>
+      <c r="D187">
+        <v>1670.17892660744</v>
+      </c>
+      <c r="E187">
+        <v>11002.4764447507</v>
+      </c>
+      <c r="F187" s="4">
+        <v>19</v>
+      </c>
+      <c r="G187">
+        <f t="shared" si="0"/>
+        <v>0.45238095238095238</v>
+      </c>
+    </row>
+    <row r="188" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A188" s="1">
+        <v>37322</v>
+      </c>
+      <c r="B188" s="1">
+        <v>9.4809921060859004E-2</v>
+      </c>
+      <c r="C188" s="1">
+        <v>84</v>
+      </c>
+      <c r="D188">
+        <v>88.323062443209395</v>
+      </c>
+      <c r="E188">
+        <v>11002.4764447507</v>
+      </c>
+      <c r="F188" s="4">
+        <v>5</v>
+      </c>
+      <c r="G188">
+        <f t="shared" si="0"/>
+        <v>5.9523809523809521E-2</v>
+      </c>
+    </row>
+    <row r="189" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A189" s="1">
+        <v>37443</v>
+      </c>
+      <c r="B189" s="1">
+        <v>1.5477801169302001E-2</v>
+      </c>
+      <c r="C189" s="1">
+        <v>27</v>
+      </c>
+      <c r="D189">
+        <v>140.19042436297801</v>
+      </c>
+      <c r="E189">
+        <v>136881.734925525</v>
+      </c>
+      <c r="F189" s="4">
+        <v>8</v>
+      </c>
+      <c r="G189">
+        <f t="shared" si="0"/>
+        <v>0.29629629629629628</v>
+      </c>
+    </row>
+    <row r="190" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A190" s="1">
+        <v>37791</v>
+      </c>
+      <c r="B190" s="1">
+        <v>0.218982084772921</v>
+      </c>
+      <c r="C190" s="1">
         <v>65</v>
       </c>
-    </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A158" s="1">
-        <v>32145</v>
-      </c>
-      <c r="B158" s="1">
-        <v>0.26118896032327898</v>
-      </c>
-      <c r="C158" s="1">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A159" s="1">
-        <v>32923</v>
-      </c>
-      <c r="B159" s="1">
-        <v>3.3038622127386001E-2</v>
-      </c>
-      <c r="C159" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A160" s="1">
-        <v>33224</v>
-      </c>
-      <c r="B160" s="1">
-        <v>8.8011013180742004E-2</v>
-      </c>
-      <c r="C160" s="1">
+      <c r="D190">
+        <v>204.52672911190001</v>
+      </c>
+      <c r="E190">
+        <v>10550.597128846501</v>
+      </c>
+      <c r="F190" s="4">
+        <v>9</v>
+      </c>
+      <c r="G190">
+        <f t="shared" si="0"/>
+        <v>0.13846153846153847</v>
+      </c>
+    </row>
+    <row r="191" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A191" s="1">
+        <v>37810</v>
+      </c>
+      <c r="B191" s="1">
+        <v>0.20975109326814401</v>
+      </c>
+      <c r="C191" s="1">
+        <v>187</v>
+      </c>
+      <c r="D191">
+        <v>243.29616927239499</v>
+      </c>
+      <c r="E191">
+        <v>14131.819344212199</v>
+      </c>
+      <c r="F191" s="4">
+        <v>2</v>
+      </c>
+      <c r="G191">
+        <f t="shared" si="0"/>
+        <v>1.06951871657754E-2</v>
+      </c>
+    </row>
+    <row r="192" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A192" s="1">
+        <v>38351</v>
+      </c>
+      <c r="B192" s="1">
+        <v>6.8016592070019996E-3</v>
+      </c>
+      <c r="C192" s="1">
+        <v>3</v>
+      </c>
+      <c r="D192">
+        <v>1710.6117362085199</v>
+      </c>
+      <c r="E192">
+        <v>6190.81488022961</v>
+      </c>
+      <c r="F192" s="4">
+        <v>3</v>
+      </c>
+      <c r="G192">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="193" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A193" s="1">
+        <v>38500</v>
+      </c>
+      <c r="B193" s="1">
+        <v>0.18482509779820899</v>
+      </c>
+      <c r="C193" s="1">
+        <v>32</v>
+      </c>
+      <c r="D193">
+        <v>834.65117130227804</v>
+      </c>
+      <c r="E193">
+        <v>85063.403566940295</v>
+      </c>
+      <c r="F193" s="4">
+        <v>32</v>
+      </c>
+      <c r="G193">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="194" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A194" s="1">
+        <v>39160</v>
+      </c>
+      <c r="B194" s="1">
+        <v>0.13596581802382701</v>
+      </c>
+      <c r="C194" s="1">
+        <v>21</v>
+      </c>
+      <c r="D194">
+        <v>777.00486220885898</v>
+      </c>
+      <c r="E194">
+        <v>36948.275038289001</v>
+      </c>
+      <c r="F194" s="4">
+        <v>21</v>
+      </c>
+      <c r="G194">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="195" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A195" s="1">
+        <v>39163</v>
+      </c>
+      <c r="B195" s="1">
+        <v>0.15852268042447901</v>
+      </c>
+      <c r="C195" s="1">
         <v>29</v>
       </c>
-    </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A161" s="1">
-        <v>33327</v>
-      </c>
-      <c r="B161" s="1">
-        <v>0.178798741068562</v>
-      </c>
-      <c r="C161" s="1">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A162" s="1">
-        <v>33340</v>
-      </c>
-      <c r="B162" s="1">
-        <v>0.18296331444587</v>
-      </c>
-      <c r="C162" s="1">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A163" s="1">
-        <v>33411</v>
-      </c>
-      <c r="B163" s="1">
-        <v>0.21607189799624801</v>
-      </c>
-      <c r="C163" s="1">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A164" s="1">
-        <v>33444</v>
-      </c>
-      <c r="B164" s="1">
-        <v>0.172066365078858</v>
-      </c>
-      <c r="C164" s="1">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A165" s="1">
-        <v>33594</v>
-      </c>
-      <c r="B165" s="1">
-        <v>0.111333339450349</v>
-      </c>
-      <c r="C165" s="1">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A166" s="1">
-        <v>33724</v>
-      </c>
-      <c r="B166" s="1">
-        <v>0.17067917439993199</v>
-      </c>
-      <c r="C166" s="1">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A167" s="1">
-        <v>33993</v>
-      </c>
-      <c r="B167" s="1">
-        <v>8.8290035277060003E-2</v>
-      </c>
-      <c r="C167" s="1">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A168" s="1">
-        <v>34175</v>
-      </c>
-      <c r="B168" s="1">
-        <v>9.3843243701032003E-2</v>
-      </c>
-      <c r="C168" s="1">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A169" s="1">
-        <v>34259</v>
-      </c>
-      <c r="B169" s="1">
-        <v>0</v>
-      </c>
-      <c r="C169" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A170" s="1">
-        <v>34261</v>
-      </c>
-      <c r="B170" s="1">
-        <v>0.137780482898372</v>
-      </c>
-      <c r="C170" s="1">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A171" s="1">
-        <v>34478</v>
-      </c>
-      <c r="B171" s="1">
-        <v>8.1211043079211995E-2</v>
-      </c>
-      <c r="C171" s="1">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A172" s="1">
-        <v>34559</v>
-      </c>
-      <c r="B172" s="1">
-        <v>1.8046923079220001E-3</v>
-      </c>
-      <c r="C172" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A173" s="1">
-        <v>34938</v>
-      </c>
-      <c r="B173" s="1">
-        <v>7.5033906778769005E-2</v>
-      </c>
-      <c r="C173" s="1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A174" s="1">
-        <v>35028</v>
-      </c>
-      <c r="B174" s="1">
-        <v>1.7977621312515998E-2</v>
-      </c>
-      <c r="C174" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A175" s="1">
-        <v>35571</v>
-      </c>
-      <c r="B175" s="1">
-        <v>0.17491835876145401</v>
-      </c>
-      <c r="C175" s="1">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A176" s="1">
-        <v>35687</v>
-      </c>
-      <c r="B176" s="1">
-        <v>0.14465490386308799</v>
-      </c>
-      <c r="C176" s="1">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A177" s="1">
-        <v>35696</v>
-      </c>
-      <c r="B177" s="1">
-        <v>0.14972198637044401</v>
-      </c>
-      <c r="C177" s="1">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A178" s="1">
-        <v>35880</v>
-      </c>
-      <c r="B178" s="1">
-        <v>0.19317438993014999</v>
-      </c>
-      <c r="C178" s="1">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A179" s="1">
-        <v>36067</v>
-      </c>
-      <c r="B179" s="1">
-        <v>0.13188361426071599</v>
-      </c>
-      <c r="C179" s="1">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A180" s="1">
-        <v>36116</v>
-      </c>
-      <c r="B180" s="1">
-        <v>0.139727217499582</v>
-      </c>
-      <c r="C180" s="1">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A181" s="1">
-        <v>36462</v>
-      </c>
-      <c r="B181" s="1">
-        <v>2.1240321393725E-2</v>
-      </c>
-      <c r="C181" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A182" s="1">
-        <v>36734</v>
-      </c>
-      <c r="B182" s="1">
-        <v>0.15005624460401901</v>
-      </c>
-      <c r="C182" s="1">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A183" s="1">
-        <v>36795</v>
-      </c>
-      <c r="B183" s="1">
-        <v>0.102513106267262</v>
-      </c>
-      <c r="C183" s="1">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A184" s="1">
-        <v>36836</v>
-      </c>
-      <c r="B184" s="1">
-        <v>0.13263552081795699</v>
-      </c>
-      <c r="C184" s="1">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A185" s="1">
-        <v>36909</v>
-      </c>
-      <c r="B185" s="1">
-        <v>0.110217403406246</v>
-      </c>
-      <c r="C185" s="1">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A186" s="1">
-        <v>37163</v>
-      </c>
-      <c r="B186" s="1">
-        <v>0.24264602874948901</v>
-      </c>
-      <c r="C186" s="1">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A187" s="1">
-        <v>37232</v>
-      </c>
-      <c r="B187" s="1">
-        <v>0.26548117389012899</v>
-      </c>
-      <c r="C187" s="1">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A188" s="1">
-        <v>37263</v>
-      </c>
-      <c r="B188" s="1">
-        <v>0.12555705320819499</v>
-      </c>
-      <c r="C188" s="1">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A189" s="1">
-        <v>37263</v>
-      </c>
-      <c r="B189" s="1">
-        <v>0.12555705320819499</v>
-      </c>
-      <c r="C189" s="1">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A190" s="1">
-        <v>37322</v>
-      </c>
-      <c r="B190" s="1">
-        <v>9.4809921060859004E-2</v>
-      </c>
-      <c r="C190" s="1">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A191" s="1">
-        <v>37443</v>
-      </c>
-      <c r="B191" s="1">
-        <v>1.5477801169302001E-2</v>
-      </c>
-      <c r="C191" s="1">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A192" s="1">
-        <v>37791</v>
-      </c>
-      <c r="B192" s="1">
-        <v>0.218982084772921</v>
-      </c>
-      <c r="C192" s="1">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A193" s="1">
-        <v>37810</v>
-      </c>
-      <c r="B193" s="1">
-        <v>0.20975109326814401</v>
-      </c>
-      <c r="C193" s="1">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A194" s="1">
-        <v>38351</v>
-      </c>
-      <c r="B194" s="1">
-        <v>6.8016592070019996E-3</v>
-      </c>
-      <c r="C194" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A195" s="1">
-        <v>38500</v>
-      </c>
-      <c r="B195" s="1">
-        <v>0.18482509779820899</v>
-      </c>
-      <c r="C195" s="1">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A196" s="1">
-        <v>39160</v>
-      </c>
-      <c r="B196" s="1">
-        <v>0.13596581802382701</v>
-      </c>
-      <c r="C196" s="1">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A197" s="1">
-        <v>39163</v>
-      </c>
-      <c r="B197" s="1">
-        <v>0.15852268042447901</v>
-      </c>
-      <c r="C197" s="1">
-        <v>29</v>
+      <c r="D195">
+        <v>23.697874934460899</v>
+      </c>
+      <c r="E195">
+        <v>9247.5623242720903</v>
+      </c>
+      <c r="F195" s="4">
+        <v>24</v>
+      </c>
+      <c r="G195">
+        <f t="shared" si="0"/>
+        <v>0.82758620689655171</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C197">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C195">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>